<commit_message>
add new part: within
</commit_message>
<xml_diff>
--- a/Ontologies/within_the_sea.xlsx
+++ b/Ontologies/within_the_sea.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="772">
   <si>
     <t>Mountain Range</t>
   </si>
@@ -1810,6 +1810,531 @@
   </si>
   <si>
     <t>east of Mountsunny</t>
+  </si>
+  <si>
+    <t>within the sea</t>
+  </si>
+  <si>
+    <t>海内经</t>
+  </si>
+  <si>
+    <t>within</t>
+  </si>
+  <si>
+    <t>the East Sea</t>
+  </si>
+  <si>
+    <t>东海</t>
+  </si>
+  <si>
+    <t>at the corner of</t>
+  </si>
+  <si>
+    <t>the North Sea</t>
+  </si>
+  <si>
+    <t>北海</t>
+  </si>
+  <si>
+    <t>Dawnfresh</t>
+  </si>
+  <si>
+    <t>Skypoison</t>
+  </si>
+  <si>
+    <t>天毒</t>
+  </si>
+  <si>
+    <t>live on the water 水居 cuddle each other sensuously and are very amorous偎人爱之</t>
+  </si>
+  <si>
+    <t>the West Sea</t>
+  </si>
+  <si>
+    <t>西海</t>
+  </si>
+  <si>
+    <t>the Flowing Sands</t>
+  </si>
+  <si>
+    <t>Chasmmarket country</t>
+  </si>
+  <si>
+    <t>壑市</t>
+  </si>
+  <si>
+    <t>Floodleaf country</t>
+  </si>
+  <si>
+    <t>泛叶</t>
+  </si>
+  <si>
+    <t>Mount Bird</t>
+  </si>
+  <si>
+    <t>鸟山</t>
+  </si>
+  <si>
+    <t>Three rivers</t>
+  </si>
+  <si>
+    <t>三水</t>
+  </si>
+  <si>
+    <t>River Liking</t>
+  </si>
+  <si>
+    <t>好人</t>
+  </si>
+  <si>
+    <t>Mount Evens</t>
+  </si>
+  <si>
+    <t>淮山</t>
+  </si>
+  <si>
+    <t>River Black</t>
+  </si>
+  <si>
+    <t>黑水</t>
+  </si>
+  <si>
+    <t>the Country of Dawncloud</t>
+  </si>
+  <si>
+    <t>朝云之国</t>
+  </si>
+  <si>
+    <t>the Country of Ruleswine</t>
+  </si>
+  <si>
+    <t>司彘之国</t>
+  </si>
+  <si>
+    <t>Mount Neverdie</t>
+  </si>
+  <si>
+    <t>不死之山</t>
+  </si>
+  <si>
+    <t>along</t>
+  </si>
+  <si>
+    <t>黑水之闲</t>
+  </si>
+  <si>
+    <t>Mount Limit</t>
+  </si>
+  <si>
+    <t>肇山</t>
+  </si>
+  <si>
+    <t>Mount Blossom</t>
+  </si>
+  <si>
+    <t>华山</t>
+  </si>
+  <si>
+    <t>River Green</t>
+  </si>
+  <si>
+    <t>青水</t>
+  </si>
+  <si>
+    <t>Cypress Tall</t>
+  </si>
+  <si>
+    <t>柏高</t>
+  </si>
+  <si>
+    <t>goes up on high from the mountain and comes back down it again，and he reaches right up into the sky上下于此，至于天</t>
+  </si>
+  <si>
+    <t>the Wilderness of Citybreadth</t>
+  </si>
+  <si>
+    <t>都广之野</t>
+  </si>
+  <si>
+    <t>the Divine Wind Bird</t>
+  </si>
+  <si>
+    <t>凤鸟</t>
+  </si>
+  <si>
+    <t>sing freely自歌</t>
+  </si>
+  <si>
+    <t>dance freely 自舞</t>
+  </si>
+  <si>
+    <t>hundred animals</t>
+  </si>
+  <si>
+    <t>百兽</t>
+  </si>
+  <si>
+    <t>the Country of Apemid</t>
+  </si>
+  <si>
+    <t>禺中之国</t>
+  </si>
+  <si>
+    <t>the Country of Rangeriseover</t>
+  </si>
+  <si>
+    <t>列襄之国</t>
+  </si>
+  <si>
+    <t>Mount Divinepower</t>
+  </si>
+  <si>
+    <t>灵山</t>
+  </si>
+  <si>
+    <t>wriggler-snake</t>
+  </si>
+  <si>
+    <t>耎蛇</t>
+  </si>
+  <si>
+    <t>scarlet</t>
+  </si>
+  <si>
+    <t>live up in trees在木上 feed on trees木食</t>
+  </si>
+  <si>
+    <t>the country of Saltlong</t>
+  </si>
+  <si>
+    <t>盐长之国</t>
+  </si>
+  <si>
+    <t>Bird Clan</t>
+  </si>
+  <si>
+    <t>鸟氏</t>
+  </si>
+  <si>
+    <t>the Mound of Pottery Superb</t>
+  </si>
+  <si>
+    <t>the Mound of Reap Get</t>
+  </si>
+  <si>
+    <t>the Mound of Chief Full</t>
+  </si>
+  <si>
+    <t>the Mound of Offspring My</t>
+  </si>
+  <si>
+    <t>the Mound of Black White</t>
+  </si>
+  <si>
+    <t>the Mound of Scarlet Watch</t>
+  </si>
+  <si>
+    <t>the Mound of Trial Guard</t>
+  </si>
+  <si>
+    <t>the Mound of Warrior Man</t>
+  </si>
+  <si>
+    <t>the Mound of the God Folk</t>
+  </si>
+  <si>
+    <t>陶唐之丘</t>
+  </si>
+  <si>
+    <t>叔得之丘</t>
+  </si>
+  <si>
+    <t>孟盈之丘</t>
+  </si>
+  <si>
+    <t>昆吾之丘</t>
+  </si>
+  <si>
+    <t>黑白之丘</t>
+  </si>
+  <si>
+    <t>赤望之丘</t>
+  </si>
+  <si>
+    <t>参卫之丘</t>
+  </si>
+  <si>
+    <t>武夫之丘</t>
+  </si>
+  <si>
+    <t>神民之丘</t>
+  </si>
+  <si>
+    <t>eat human食人</t>
+  </si>
+  <si>
+    <t>live-lively</t>
+  </si>
+  <si>
+    <t>猩猩</t>
+  </si>
+  <si>
+    <t>Bigsnake Country</t>
+  </si>
+  <si>
+    <t>巴国</t>
+  </si>
+  <si>
+    <t>流黄辛氏</t>
+  </si>
+  <si>
+    <t>the country of Flowingyellow-bitterclan</t>
+  </si>
+  <si>
+    <t>Mount Bigsnake-follow</t>
+  </si>
+  <si>
+    <t>巴遂山</t>
+  </si>
+  <si>
+    <t>River Rope</t>
+  </si>
+  <si>
+    <t>渑水</t>
+  </si>
+  <si>
+    <t>the country of Crimsonroll</t>
+  </si>
+  <si>
+    <t>朱卷之国</t>
+  </si>
+  <si>
+    <t>black snake</t>
+  </si>
+  <si>
+    <t>黑蛇</t>
+  </si>
+  <si>
+    <t>eat elephant</t>
+  </si>
+  <si>
+    <t>the Giants of the Land of Tribute</t>
+  </si>
+  <si>
+    <t>赣巨人</t>
+  </si>
+  <si>
+    <t>long forearms 长臂 hairy 有毛 heels are back-to-front反踵 when see people they laugh and laugh见人笑亦笑 lips cover their whole face 唇蔽其面，this is how other people make their escape from the giants因即逃也</t>
+  </si>
+  <si>
+    <t>Black people</t>
+  </si>
+  <si>
+    <t>黑人</t>
+  </si>
+  <si>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>both hands hold snakes两手持蛇 chewing on snakes 方啗之</t>
+  </si>
+  <si>
+    <t>the land of Full Folk</t>
+  </si>
+  <si>
+    <t>嬴民</t>
+  </si>
+  <si>
+    <t>boundary-boar</t>
+  </si>
+  <si>
+    <t>封豕</t>
+  </si>
+  <si>
+    <t>the Sprout Folk</t>
+  </si>
+  <si>
+    <t>苗民</t>
+  </si>
+  <si>
+    <t>sing freely</t>
+  </si>
+  <si>
+    <t>dance freely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>head markings ‘Virtue’,wing markings 'Obedience',chest 'Humaniy', back ' Justice'首文曰德翼文曰顺膺文曰仁背文曰义</t>
+  </si>
+  <si>
+    <t>harmony 天下和</t>
+  </si>
+  <si>
+    <t>mushroom-dog</t>
+  </si>
+  <si>
+    <t>𡹤狗</t>
+  </si>
+  <si>
+    <t>hare菟</t>
+  </si>
+  <si>
+    <t>kingfisher</t>
+  </si>
+  <si>
+    <t>翠鸟</t>
+  </si>
+  <si>
+    <t>peacock</t>
+  </si>
+  <si>
+    <t>孔鸟</t>
+  </si>
+  <si>
+    <t>Mount Balance</t>
+  </si>
+  <si>
+    <t>Mount Mushroom</t>
+  </si>
+  <si>
+    <t>Mount Cinnamon</t>
+  </si>
+  <si>
+    <t>衡山</t>
+  </si>
+  <si>
+    <t>菌山</t>
+  </si>
+  <si>
+    <t>桂山</t>
+  </si>
+  <si>
+    <t>the South Sea</t>
+  </si>
+  <si>
+    <t>南海</t>
+  </si>
+  <si>
+    <t>三天子之都</t>
+  </si>
+  <si>
+    <t>Mound of the Blueplanetree</t>
+  </si>
+  <si>
+    <t>苍梧之丘</t>
+  </si>
+  <si>
+    <t>Mount Snake</t>
+  </si>
+  <si>
+    <t>蛇山</t>
+  </si>
+  <si>
+    <t>River Snake</t>
+  </si>
+  <si>
+    <t>蛇水</t>
+  </si>
+  <si>
+    <t>the screen bird</t>
+  </si>
+  <si>
+    <t>翳鸟</t>
+  </si>
+  <si>
+    <t>multicolored</t>
+  </si>
+  <si>
+    <t>when flies it blankets the whole contryside 飞蔽一乡</t>
+  </si>
+  <si>
+    <t>Mount Nospur</t>
+  </si>
+  <si>
+    <t>不距之山</t>
+  </si>
+  <si>
+    <t>Baseherder land</t>
+  </si>
+  <si>
+    <t>氐羌</t>
+  </si>
+  <si>
+    <t>Beg as family name乞姓</t>
+  </si>
+  <si>
+    <t>Mount Gloomycity</t>
+  </si>
+  <si>
+    <t>幽都之山</t>
+  </si>
+  <si>
+    <t>dark bird</t>
+  </si>
+  <si>
+    <t>dark snake</t>
+  </si>
+  <si>
+    <t>dark panther</t>
+  </si>
+  <si>
+    <t>dark tiger</t>
+  </si>
+  <si>
+    <t>dark fox</t>
+  </si>
+  <si>
+    <t>bushy tail 蓬尾</t>
+  </si>
+  <si>
+    <t>玄鸟</t>
+  </si>
+  <si>
+    <t>玄蛇</t>
+  </si>
+  <si>
+    <t>玄豹</t>
+  </si>
+  <si>
+    <t>玄虎</t>
+  </si>
+  <si>
+    <t>玄狐</t>
+  </si>
+  <si>
+    <t>Mount Bigdark</t>
+  </si>
+  <si>
+    <t>大玄之山</t>
+  </si>
+  <si>
+    <t>Darkmound Folk</t>
+  </si>
+  <si>
+    <t>玄丘之民</t>
+  </si>
+  <si>
+    <t>the Country of Biggloom</t>
+  </si>
+  <si>
+    <t>大幽之国</t>
+  </si>
+  <si>
+    <t>Scarletlegs Folk</t>
+  </si>
+  <si>
+    <t>赤胫之民</t>
+  </si>
+  <si>
+    <t>the Country of Pegdivinepower</t>
+  </si>
+  <si>
+    <t>钉灵之国</t>
+  </si>
+  <si>
+    <t>hairy from the knees down从膝下已有毛 horse‘s hoof马蹄 fine runners善走</t>
   </si>
 </sst>
 </file>
@@ -2154,10 +2679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EE151"/>
+  <dimension ref="A1:EE217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q125" workbookViewId="0">
-      <selection activeCell="Z150" sqref="Z150:AA151"/>
+    <sheetView tabSelected="1" topLeftCell="DT194" workbookViewId="0">
+      <selection activeCell="DW217" sqref="DW217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2166,15 +2691,16 @@
     <col min="3" max="3" width="19.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="30.21875" style="2" customWidth="1"/>
     <col min="5" max="6" width="16.6640625" style="2"/>
-    <col min="7" max="7" width="30.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" style="2" customWidth="1"/>
     <col min="8" max="13" width="16.6640625" style="2"/>
     <col min="14" max="14" width="25.21875" style="2" customWidth="1"/>
     <col min="15" max="16" width="16.6640625" style="2"/>
     <col min="17" max="17" width="20.44140625" style="2" customWidth="1"/>
     <col min="18" max="20" width="16.6640625" style="2"/>
     <col min="21" max="21" width="23.109375" style="2" customWidth="1"/>
-    <col min="22" max="24" width="16.6640625" style="2"/>
-    <col min="25" max="25" width="22.109375" style="2" customWidth="1"/>
+    <col min="22" max="23" width="16.6640625" style="2"/>
+    <col min="24" max="24" width="17.21875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="27.33203125" style="2" customWidth="1"/>
     <col min="26" max="104" width="16.6640625" style="2"/>
     <col min="105" max="105" width="34" style="2" customWidth="1"/>
     <col min="106" max="126" width="16.6640625" style="2"/>
@@ -5622,7 +6148,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="145" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q145" s="2" t="s">
         <v>559</v>
       </c>
@@ -5654,7 +6180,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="146" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q146" s="2" t="s">
         <v>563</v>
       </c>
@@ -5686,7 +6212,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="147" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q147" s="2" t="s">
         <v>571</v>
       </c>
@@ -5718,7 +6244,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="148" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q148" s="2" t="s">
         <v>576</v>
       </c>
@@ -5747,7 +6273,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="149" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q149" s="2" t="s">
         <v>581</v>
       </c>
@@ -5776,7 +6302,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="150" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q150" s="2" t="s">
         <v>587</v>
       </c>
@@ -5808,7 +6334,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="151" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:127" x14ac:dyDescent="0.3">
       <c r="Q151" s="2" t="s">
         <v>593</v>
       </c>
@@ -5838,6 +6364,1047 @@
       </c>
       <c r="AA151" s="2" t="s">
         <v>592</v>
+      </c>
+    </row>
+    <row r="152" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="K152" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N152" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="O152" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="153" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="K153" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="N153" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="O153" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="154" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="G154" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="K154" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N154" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="O154" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="Y154" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="Z154" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA154" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DW154" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="155" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="K155" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="N155" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="O155" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="156" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="G156" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="K156" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="O156" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="157" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="K157" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N157" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O157" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="158" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="G158" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="K158" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N158" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="O158" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="159" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="K159" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N159" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O159" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="160" spans="1:127" x14ac:dyDescent="0.3">
+      <c r="D160" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="K160" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N160" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O160" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q160" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="R160" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="U160" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V160" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="161" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D161" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q161" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="R161" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="U161" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="V161" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="162" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G162" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="K162" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N162" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O162" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="163" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="K163" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N163" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="O163" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="164" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G164" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="K164" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N164" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O164" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="165" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="K165" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N165" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="O165" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="166" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D166" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K166" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N166" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="O166" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="167" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="K167" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="N167" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="O167" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="168" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D168" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="O168" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="Y168" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="Z168" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="AA168" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DW168" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="169" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="K169" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N169" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="O169" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="170" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D170" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="K170" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="O170" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="Y170" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z170" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA170" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW170" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="171" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="K171" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="O171" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="Y171" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="Z171" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="AA171" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW171" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="172" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y172" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="Z172" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="AA172" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="173" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G173" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="174" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G174" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="175" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D175" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="Y175" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="Z175" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="AA175" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AS175" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="DW175" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="176" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G176" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="Y176" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z176" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA176" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BM176" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="177" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D177" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="178" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D178" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="179" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D179" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="180" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D180" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="181" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D181" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="182" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D182" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="183" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D183" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="184" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D184" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="185" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D185" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="186" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G186" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y186" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z186" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA186" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="BM186" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DW186" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="187" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y187" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="Z187" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AA187" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AS187" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AY187" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="188" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G188" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="189" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D189" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q189" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="R189" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="190" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G190" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y190" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="Z190" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="AA190" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="BJ190" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="DW190" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="191" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G191" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y191" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="Z191" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA191" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS191" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY191" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DW191" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="192" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G192" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="Y192" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="Z192" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="AA192" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BM192" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="BY192" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW192" s="2" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="193" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="G193" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="H193" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="Y193" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="Z193" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="AA193" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BY193" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="194" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y194" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="Z194" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="AA194" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="195" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="G195" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="Y195" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="Z195" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="AA195" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="196" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y196" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z196" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA196" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW196" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="197" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y197" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z197" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="AA197" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW197" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="DX197" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="EE197" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="198" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y198" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="Z198" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="AA198" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC198" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="AS198" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="DX198" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="199" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y199" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="Z199" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA199" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="200" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="Y200" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="Z200" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="AA200" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="201" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D201" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="K201" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N201" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="O201" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="202" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D202" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="K202" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N202" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="O202" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="203" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D203" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="K203" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N203" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="O203" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="204" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D204" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="K204" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N204" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="O204" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="205" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D205" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="206" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D206" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="K206" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N206" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="O206" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q206" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="R206" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="U206" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="V206" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="Y206" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="Z206" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA206" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AS206" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="DW206" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="207" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="D207" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="208" spans="4:135" x14ac:dyDescent="0.3">
+      <c r="G208" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="Y208" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="Z208" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="AA208" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DW208" s="2" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="209" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D209" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="K209" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N209" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="O209" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q209" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="R209" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="Y209" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="Z209" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="AA209" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="210" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y210" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="Z210" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="AA210" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="211" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y211" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="Z211" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="AA211" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="212" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y212" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="Z212" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="AA212" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="213" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="Y213" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="Z213" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="AA213" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DW213" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="214" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="D214" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="G214" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="215" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G215" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="216" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G216" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="H216" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="217" spans="4:127" x14ac:dyDescent="0.3">
+      <c r="G217" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="Y217" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="Z217" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="AA217" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DW217" s="2" t="s">
+        <v>771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>